<commit_message>
added photo to excel option
</commit_message>
<xml_diff>
--- a/day1.xlsx
+++ b/day1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshbeehler/Documents/gabba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E83A2C1-C4BB-1F45-AC4E-1208E451CD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA99B503-60CE-1C46-B0C8-9BD45EA20D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15560" xr2:uid="{5C5AEA5A-01B2-434D-8FAB-79E3919C3C72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="25">
   <si>
     <t>Box</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>7:15pm</t>
+  </si>
+  <si>
+    <t>7+A3</t>
   </si>
 </sst>
 </file>
@@ -488,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89F224B-7C3B-D34D-9475-0ED745590AC7}">
   <dimension ref="A1:F331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="H325" sqref="H325"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,8 +518,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3211</v>
+      <c r="A2" t="s">
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>

</xml_diff>